<commit_message>
fix: Header css so font is white
</commit_message>
<xml_diff>
--- a/bugs-db.xlsx
+++ b/bugs-db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buckey/Documents/learning/mean-dev/Loc8r/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7028F3-7239-9C42-9E10-7624D9FD9596}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5298B51-16BE-9A4C-BE8B-F406C7A7FC1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23880" yWindow="9900" windowWidth="17520" windowHeight="19060" xr2:uid="{A6442886-FAE9-014C-A8CE-D1493FC986CE}"/>
+    <workbookView xWindow="-27180" yWindow="-12940" windowWidth="17520" windowHeight="19060" xr2:uid="{A6442886-FAE9-014C-A8CE-D1493FC986CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Leo</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Header Bar Hidding Content</t>
+  </si>
+  <si>
+    <t>Header Blocks first element of Locations List</t>
+  </si>
+  <si>
+    <t>First Location in list of loactions should be displayed below header nav</t>
   </si>
 </sst>
 </file>
@@ -418,7 +430,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,14 +476,26 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: add homepage component to encapsule Loc8r app homepage
</commit_message>
<xml_diff>
--- a/bugs-db.xlsx
+++ b/bugs-db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buckey/Documents/learning/mean-dev/Loc8r/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5298B51-16BE-9A4C-BE8B-F406C7A7FC1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC094AA3-92D1-1345-B397-9D25D6CF9366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27180" yWindow="-12940" windowWidth="17520" windowHeight="19060" xr2:uid="{A6442886-FAE9-014C-A8CE-D1493FC986CE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -496,7 +496,9 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>

</xml_diff>